<commit_message>
feat(puppeteer):save the group to chat
</commit_message>
<xml_diff>
--- a/chats/34603358135@c.us.xlsx
+++ b/chats/34603358135@c.us.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Fecha</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Por donde va mi pedido</t>
+  </si>
+  <si>
+    <t>28-02-2023 04:12</t>
+  </si>
+  <si>
+    <t>hola</t>
   </si>
 </sst>
 </file>
@@ -429,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -504,6 +510,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>